<commit_message>
Added Support for multiple IPs, as well as File IO
</commit_message>
<xml_diff>
--- a/Report T400 400E.xlsx
+++ b/Report T400 400E.xlsx
@@ -747,8 +747,8 @@
   </sheetPr>
   <dimension ref="B1:M38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28:G28"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" topLeftCell="A13" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>